<commit_message>
- Update Data (1 additional respondent) - Update R Markdown Prolific
</commit_message>
<xml_diff>
--- a/Data_EE Downward Causation_Conjoint_Wave3.xlsx
+++ b/Data_EE Downward Causation_Conjoint_Wave3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johannes.haehnlein\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johannes.haehnlein\Desktop\Johannes Haehnlein\19_PROMOTION\01_STUDIEN\Studie 2 - Conjoint\Data\R Repository\EE_Downward-Causation_Entrepreneurship-Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32E704E-03B3-4057-B6B4-5064799CD857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6142FBC6-3F5F-4689-8493-386A805D0F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studie zur Stärkung von Gründun" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="140">
   <si>
     <t>age</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Heidelberg</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Darmstadt</t>
@@ -448,6 +445,15 @@
   <si>
     <t>duration</t>
   </si>
+  <si>
+    <t>Ludwigshafen</t>
+  </si>
+  <si>
+    <t>Hofheim</t>
+  </si>
+  <si>
+    <t>Kassel</t>
+  </si>
 </sst>
 </file>
 
@@ -481,10 +487,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -799,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ116"/>
+  <dimension ref="A1:BZ117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BV1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CE19" sqref="CE19"/>
+    <sheetView tabSelected="1" topLeftCell="Q79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z103" sqref="Z103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -867,193 +874,193 @@
         <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Y1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="BC1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BE1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BF1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="BF1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="BI1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="BJ1" s="2" t="s">
+      <c r="BK1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="BK1" s="2" t="s">
+      <c r="BL1" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="BL1" s="2" t="s">
+      <c r="BM1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="BM1" s="2" t="s">
+      <c r="BN1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="BN1" s="2" t="s">
+      <c r="BO1" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="BO1" s="2" t="s">
+      <c r="BP1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="BP1" s="2" t="s">
+      <c r="BQ1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="BQ1" s="2" t="s">
+      <c r="BR1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="BR1" s="2" t="s">
+      <c r="BS1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="BS1" s="2" t="s">
+      <c r="BT1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="BT1" s="2" t="s">
+      <c r="BU1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="BU1" s="2" t="s">
+      <c r="BV1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="BV1" s="2" t="s">
+      <c r="BW1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="BW1" s="2" t="s">
+      <c r="BX1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="BX1" s="2" t="s">
+      <c r="BY1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BZ1" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="BZ1" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:78" x14ac:dyDescent="0.25">
@@ -2734,7 +2741,7 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="K9">
         <v>15</v>
@@ -2970,7 +2977,7 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10">
         <v>10</v>
@@ -3206,7 +3213,7 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -3442,7 +3449,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K12">
         <v>6</v>
@@ -3914,7 +3921,7 @@
         <v>3</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14">
         <v>7</v>
@@ -4386,7 +4393,7 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K16">
         <v>4</v>
@@ -4622,7 +4629,7 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K17">
         <v>5</v>
@@ -4855,7 +4862,7 @@
         <v>0</v>
       </c>
       <c r="J18" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -5091,7 +5098,7 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K19">
         <v>4</v>
@@ -5327,7 +5334,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K20">
         <v>13</v>
@@ -5563,7 +5570,7 @@
         <v>4</v>
       </c>
       <c r="J21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K21">
         <v>5</v>
@@ -5799,7 +5806,7 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K22">
         <v>4</v>
@@ -6035,7 +6042,7 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K23">
         <v>4</v>
@@ -6268,7 +6275,7 @@
         <v>0</v>
       </c>
       <c r="J24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K24">
         <v>2</v>
@@ -6504,7 +6511,7 @@
         <v>3</v>
       </c>
       <c r="J25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K25">
         <v>12</v>
@@ -6522,19 +6529,19 @@
         <v>6</v>
       </c>
       <c r="P25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q25">
         <v>2</v>
       </c>
       <c r="R25">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S25">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="T25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U25">
         <v>4</v>
@@ -6543,34 +6550,34 @@
         <v>7</v>
       </c>
       <c r="W25">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="X25">
         <v>4</v>
       </c>
       <c r="Y25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z25">
         <v>2</v>
       </c>
       <c r="AA25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AC25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AD25">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AE25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AF25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AG25">
         <v>6</v>
@@ -6740,7 +6747,7 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K26">
         <v>4</v>
@@ -6976,7 +6983,7 @@
         <v>2</v>
       </c>
       <c r="J27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K27">
         <v>15</v>
@@ -7211,8 +7218,8 @@
       <c r="I28">
         <v>9</v>
       </c>
-      <c r="J28">
-        <v>65719</v>
+      <c r="J28" t="s">
+        <v>139</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -7684,7 +7691,7 @@
         <v>3</v>
       </c>
       <c r="J30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K30">
         <v>11</v>
@@ -7920,7 +7927,7 @@
         <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K31">
         <v>9</v>
@@ -8156,7 +8163,7 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -8392,7 +8399,7 @@
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K33">
         <v>4</v>
@@ -8628,7 +8635,7 @@
         <v>4</v>
       </c>
       <c r="J34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K34">
         <v>7</v>
@@ -8864,7 +8871,7 @@
         <v>9</v>
       </c>
       <c r="J35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K35">
         <v>5</v>
@@ -9100,7 +9107,7 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K36">
         <v>2</v>
@@ -9336,7 +9343,7 @@
         <v>4</v>
       </c>
       <c r="J37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K37">
         <v>5</v>
@@ -9805,7 +9812,7 @@
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -10041,7 +10048,7 @@
         <v>2</v>
       </c>
       <c r="J40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K40">
         <v>4</v>
@@ -10510,7 +10517,7 @@
         <v>4</v>
       </c>
       <c r="J42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K42">
         <v>4</v>
@@ -10746,7 +10753,7 @@
         <v>7</v>
       </c>
       <c r="J43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K43">
         <v>10</v>
@@ -10979,7 +10986,7 @@
         <v>0</v>
       </c>
       <c r="J44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K44">
         <v>23</v>
@@ -11215,7 +11222,7 @@
         <v>2</v>
       </c>
       <c r="J45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K45">
         <v>12</v>
@@ -11451,7 +11458,7 @@
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K46">
         <v>2</v>
@@ -11687,7 +11694,7 @@
         <v>9</v>
       </c>
       <c r="J47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K47">
         <v>6</v>
@@ -11923,7 +11930,7 @@
         <v>5</v>
       </c>
       <c r="J48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K48">
         <v>3</v>
@@ -12159,7 +12166,7 @@
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K49">
         <v>3</v>
@@ -12395,7 +12402,7 @@
         <v>5</v>
       </c>
       <c r="J50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K50">
         <v>3</v>
@@ -12631,7 +12638,7 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K51">
         <v>4</v>
@@ -12867,7 +12874,7 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K52">
         <v>14</v>
@@ -13103,7 +13110,7 @@
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K53">
         <v>2</v>
@@ -13339,7 +13346,7 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -13575,7 +13582,7 @@
         <v>9</v>
       </c>
       <c r="J55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K55">
         <v>40</v>
@@ -13811,7 +13818,7 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K56">
         <v>3</v>
@@ -14044,7 +14051,7 @@
         <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K57">
         <v>3</v>
@@ -14277,7 +14284,7 @@
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K58">
         <v>20</v>
@@ -14513,7 +14520,7 @@
         <v>3</v>
       </c>
       <c r="J59" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K59">
         <v>10</v>
@@ -14749,7 +14756,7 @@
         <v>6</v>
       </c>
       <c r="J60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K60">
         <v>5</v>
@@ -15221,7 +15228,7 @@
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K62">
         <v>7</v>
@@ -15457,7 +15464,7 @@
         <v>6</v>
       </c>
       <c r="J63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -15693,7 +15700,7 @@
         <v>1</v>
       </c>
       <c r="J64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K64">
         <v>4</v>
@@ -15929,7 +15936,7 @@
         <v>1</v>
       </c>
       <c r="J65" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K65">
         <v>2</v>
@@ -16162,7 +16169,7 @@
         <v>0</v>
       </c>
       <c r="J66" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K66">
         <v>2</v>
@@ -16398,7 +16405,7 @@
         <v>1</v>
       </c>
       <c r="J67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K67">
         <v>0</v>
@@ -16634,7 +16641,7 @@
         <v>4</v>
       </c>
       <c r="J68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K68">
         <v>3</v>
@@ -16870,7 +16877,7 @@
         <v>1</v>
       </c>
       <c r="J69" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K69">
         <v>7</v>
@@ -17103,7 +17110,7 @@
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -17339,7 +17346,7 @@
         <v>7</v>
       </c>
       <c r="J71" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K71">
         <v>7</v>
@@ -17575,7 +17582,7 @@
         <v>1</v>
       </c>
       <c r="J72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K72">
         <v>2</v>
@@ -17811,7 +17818,7 @@
         <v>1</v>
       </c>
       <c r="J73" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K73">
         <v>0</v>
@@ -18047,7 +18054,7 @@
         <v>5</v>
       </c>
       <c r="J74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K74">
         <v>5</v>
@@ -18283,7 +18290,7 @@
         <v>4</v>
       </c>
       <c r="J75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K75">
         <v>32</v>
@@ -18519,7 +18526,7 @@
         <v>1</v>
       </c>
       <c r="J76" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K76">
         <v>12</v>
@@ -18755,7 +18762,7 @@
         <v>2</v>
       </c>
       <c r="J77" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K77">
         <v>20</v>
@@ -18991,7 +18998,7 @@
         <v>1</v>
       </c>
       <c r="J78" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K78">
         <v>2</v>
@@ -19227,7 +19234,7 @@
         <v>2</v>
       </c>
       <c r="J79" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K79">
         <v>4</v>
@@ -19463,7 +19470,7 @@
         <v>2</v>
       </c>
       <c r="J80" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K80">
         <v>38</v>
@@ -19699,7 +19706,7 @@
         <v>2</v>
       </c>
       <c r="J81" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K81">
         <v>9</v>
@@ -19935,7 +19942,7 @@
         <v>1</v>
       </c>
       <c r="J82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K82">
         <v>22</v>
@@ -20171,7 +20178,7 @@
         <v>1</v>
       </c>
       <c r="J83" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K83">
         <v>0</v>
@@ -20407,7 +20414,7 @@
         <v>3</v>
       </c>
       <c r="J84" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K84">
         <v>15</v>
@@ -20643,7 +20650,7 @@
         <v>1</v>
       </c>
       <c r="J85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K85">
         <v>15</v>
@@ -20879,7 +20886,7 @@
         <v>2</v>
       </c>
       <c r="J86" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K86">
         <v>5</v>
@@ -21115,7 +21122,7 @@
         <v>1</v>
       </c>
       <c r="J87" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K87">
         <v>6</v>
@@ -21351,7 +21358,7 @@
         <v>1</v>
       </c>
       <c r="J88" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K88">
         <v>0</v>
@@ -21587,7 +21594,7 @@
         <v>1</v>
       </c>
       <c r="J89" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K89">
         <v>34</v>
@@ -21823,7 +21830,7 @@
         <v>2</v>
       </c>
       <c r="J90" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K90">
         <v>5</v>
@@ -22059,7 +22066,7 @@
         <v>1</v>
       </c>
       <c r="J91" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K91">
         <v>4</v>
@@ -22074,7 +22081,7 @@
         <v>0</v>
       </c>
       <c r="O91" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P91">
         <v>3</v>
@@ -22295,7 +22302,7 @@
         <v>1</v>
       </c>
       <c r="J92" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K92">
         <v>1</v>
@@ -22530,8 +22537,8 @@
       <c r="I93">
         <v>1</v>
       </c>
-      <c r="J93">
-        <v>72</v>
+      <c r="J93" t="s">
+        <v>43</v>
       </c>
       <c r="K93">
         <v>40</v>
@@ -22766,8 +22773,8 @@
       <c r="I94">
         <v>7</v>
       </c>
-      <c r="J94">
-        <v>69181</v>
+      <c r="J94" t="s">
+        <v>138</v>
       </c>
       <c r="K94">
         <v>50</v>
@@ -23000,7 +23007,7 @@
         <v>0</v>
       </c>
       <c r="J95" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K95">
         <v>4</v>
@@ -23472,7 +23479,7 @@
         <v>1</v>
       </c>
       <c r="J97" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K97">
         <v>17</v>
@@ -23708,7 +23715,7 @@
         <v>1</v>
       </c>
       <c r="J98" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K98">
         <v>2</v>
@@ -23944,7 +23951,7 @@
         <v>1</v>
       </c>
       <c r="J99" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K99">
         <v>3</v>
@@ -24180,7 +24187,7 @@
         <v>1</v>
       </c>
       <c r="J100" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K100">
         <v>5</v>
@@ -24416,7 +24423,7 @@
         <v>2</v>
       </c>
       <c r="J101" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K101">
         <v>6</v>
@@ -24885,7 +24892,7 @@
         <v>1</v>
       </c>
       <c r="J103" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K103">
         <v>8</v>
@@ -25357,7 +25364,7 @@
         <v>1</v>
       </c>
       <c r="J105" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K105">
         <v>0</v>
@@ -25375,55 +25382,55 @@
         <v>6</v>
       </c>
       <c r="P105">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q105">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="T105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="U105">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W105">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X105">
         <v>4</v>
       </c>
       <c r="Y105">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z105">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AB105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AD105">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AF105">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AG105">
         <v>6</v>
@@ -25593,7 +25600,7 @@
         <v>1</v>
       </c>
       <c r="J106" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K106">
         <v>3</v>
@@ -25829,7 +25836,7 @@
         <v>5</v>
       </c>
       <c r="J107" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K107">
         <v>3</v>
@@ -26062,7 +26069,7 @@
         <v>0</v>
       </c>
       <c r="J108" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K108">
         <v>11</v>
@@ -26298,7 +26305,7 @@
         <v>1</v>
       </c>
       <c r="J109" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K109">
         <v>1</v>
@@ -26770,7 +26777,7 @@
         <v>1</v>
       </c>
       <c r="J111" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K111">
         <v>2</v>
@@ -27006,7 +27013,7 @@
         <v>2</v>
       </c>
       <c r="J112" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K112">
         <v>13</v>
@@ -27242,7 +27249,7 @@
         <v>2</v>
       </c>
       <c r="J113" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K113">
         <v>4</v>
@@ -27478,7 +27485,7 @@
         <v>6</v>
       </c>
       <c r="J114" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K114">
         <v>6</v>
@@ -27714,7 +27721,7 @@
         <v>1</v>
       </c>
       <c r="J115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K115">
         <v>6</v>
@@ -27950,7 +27957,7 @@
         <v>2</v>
       </c>
       <c r="J116" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K116">
         <v>5</v>
@@ -28155,6 +28162,242 @@
       </c>
       <c r="BZ116" s="1">
         <v>20.139833333333335</v>
+      </c>
+    </row>
+    <row r="117" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>24</v>
+      </c>
+      <c r="B117" s="2">
+        <v>2</v>
+      </c>
+      <c r="C117" s="2">
+        <v>6</v>
+      </c>
+      <c r="D117" s="2">
+        <v>2</v>
+      </c>
+      <c r="E117" s="2">
+        <v>1</v>
+      </c>
+      <c r="F117" s="2">
+        <v>1</v>
+      </c>
+      <c r="G117" s="2">
+        <v>2</v>
+      </c>
+      <c r="H117" s="2">
+        <v>1</v>
+      </c>
+      <c r="I117" s="2">
+        <v>1</v>
+      </c>
+      <c r="J117" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K117" s="2">
+        <v>0</v>
+      </c>
+      <c r="L117" s="2">
+        <v>0</v>
+      </c>
+      <c r="M117" s="2">
+        <v>1</v>
+      </c>
+      <c r="N117" s="2">
+        <v>0</v>
+      </c>
+      <c r="O117" s="2">
+        <v>6</v>
+      </c>
+      <c r="P117" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q117" s="2">
+        <v>4</v>
+      </c>
+      <c r="R117" s="2">
+        <v>5</v>
+      </c>
+      <c r="S117" s="2">
+        <v>5</v>
+      </c>
+      <c r="T117" s="2">
+        <v>4</v>
+      </c>
+      <c r="U117" s="2">
+        <v>6</v>
+      </c>
+      <c r="V117" s="2">
+        <v>3</v>
+      </c>
+      <c r="W117" s="2">
+        <v>7</v>
+      </c>
+      <c r="X117" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y117" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z117" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA117" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB117" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC117" s="2">
+        <v>4</v>
+      </c>
+      <c r="AD117" s="2">
+        <v>6</v>
+      </c>
+      <c r="AE117" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG117" s="2">
+        <v>4</v>
+      </c>
+      <c r="AH117" s="2">
+        <v>4</v>
+      </c>
+      <c r="AI117" s="2">
+        <v>2</v>
+      </c>
+      <c r="AJ117" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK117" s="2">
+        <v>5</v>
+      </c>
+      <c r="AL117" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AQ117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AR117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AS117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AU117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AV117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AW117" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AY117" s="2">
+        <v>7</v>
+      </c>
+      <c r="AZ117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BA117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BB117" s="2">
+        <v>6</v>
+      </c>
+      <c r="BC117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BD117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BE117" s="2">
+        <v>5</v>
+      </c>
+      <c r="BF117" s="2">
+        <v>5</v>
+      </c>
+      <c r="BG117" s="2">
+        <v>4</v>
+      </c>
+      <c r="BH117" s="2">
+        <v>6</v>
+      </c>
+      <c r="BI117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BJ117" s="2">
+        <v>6</v>
+      </c>
+      <c r="BK117" s="2">
+        <v>6</v>
+      </c>
+      <c r="BL117" s="2">
+        <v>4</v>
+      </c>
+      <c r="BM117" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN117" s="2">
+        <v>4</v>
+      </c>
+      <c r="BO117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BP117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BQ117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BR117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BS117" s="2">
+        <v>7</v>
+      </c>
+      <c r="BT117" s="2">
+        <v>4</v>
+      </c>
+      <c r="BU117" s="2">
+        <v>4</v>
+      </c>
+      <c r="BV117" s="2">
+        <v>5</v>
+      </c>
+      <c r="BW117" s="2">
+        <v>3</v>
+      </c>
+      <c r="BX117" s="2">
+        <v>4</v>
+      </c>
+      <c r="BY117" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ117" s="3">
+        <v>9.815666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updating manual and prolific data sets
- including model performance of multilevel models
</commit_message>
<xml_diff>
--- a/Data_EE Downward Causation_Conjoint_Wave3.xlsx
+++ b/Data_EE Downward Causation_Conjoint_Wave3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johannes.haehnlein\Desktop\Johannes Haehnlein\19_PROMOTION\01_STUDIEN\Studie 2 - Conjoint\Data\R Repository\EE_Downward-Causation_Entrepreneurship-Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6142FBC6-3F5F-4689-8493-386A805D0F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F109BAC4-DE22-4302-8BEF-61B94645690E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studie zur Stärkung von Gründun" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="142">
   <si>
     <t>age</t>
   </si>
@@ -454,6 +454,12 @@
   <si>
     <t>Kassel</t>
   </si>
+  <si>
+    <t>Köln</t>
+  </si>
+  <si>
+    <t>Göttingen</t>
+  </si>
 </sst>
 </file>
 
@@ -806,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ117"/>
+  <dimension ref="A1:BZ125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z103" sqref="Z103"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120:XFD125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -820,7 +826,9 @@
     <col min="19" max="19" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="11.44140625"/>
     <col min="27" max="27" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="40" width="11.44140625"/>
+    <col min="28" max="35" width="11.44140625"/>
+    <col min="36" max="36" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="40" width="11.44140625"/>
     <col min="41" max="41" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="42" max="71" width="11.44140625"/>
     <col min="72" max="72" width="17.88671875" bestFit="1" customWidth="1"/>
@@ -28398,6 +28406,1894 @@
       </c>
       <c r="BZ117" s="3">
         <v>9.815666666666667</v>
+      </c>
+    </row>
+    <row r="118" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>35</v>
+      </c>
+      <c r="B118" s="2">
+        <v>2</v>
+      </c>
+      <c r="C118" s="2">
+        <v>6</v>
+      </c>
+      <c r="D118" s="2">
+        <v>9</v>
+      </c>
+      <c r="E118" s="2">
+        <v>1</v>
+      </c>
+      <c r="F118" s="2">
+        <v>1</v>
+      </c>
+      <c r="G118" s="2">
+        <v>3</v>
+      </c>
+      <c r="H118" s="2">
+        <v>1</v>
+      </c>
+      <c r="I118" s="2">
+        <v>3</v>
+      </c>
+      <c r="J118" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="K118" s="2">
+        <v>23</v>
+      </c>
+      <c r="L118" s="2">
+        <v>1</v>
+      </c>
+      <c r="M118" s="2">
+        <v>1</v>
+      </c>
+      <c r="N118" s="2">
+        <v>0</v>
+      </c>
+      <c r="O118" s="2">
+        <v>6</v>
+      </c>
+      <c r="P118" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q118" s="2">
+        <v>3</v>
+      </c>
+      <c r="R118" s="2">
+        <v>5</v>
+      </c>
+      <c r="S118" s="2">
+        <v>6</v>
+      </c>
+      <c r="T118" s="2">
+        <v>4</v>
+      </c>
+      <c r="U118" s="2">
+        <v>2</v>
+      </c>
+      <c r="V118" s="2">
+        <v>2</v>
+      </c>
+      <c r="W118" s="2">
+        <v>6</v>
+      </c>
+      <c r="X118" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y118" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z118" s="2">
+        <v>2</v>
+      </c>
+      <c r="AA118" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AD118" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE118" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF118" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AH118" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI118" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ118" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AL118" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM118" s="2">
+        <v>6</v>
+      </c>
+      <c r="AN118" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AP118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AQ118" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR118" s="2">
+        <v>3</v>
+      </c>
+      <c r="AS118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AT118" s="2">
+        <v>3</v>
+      </c>
+      <c r="AU118" s="2">
+        <v>6</v>
+      </c>
+      <c r="AV118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AW118" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX118" s="2">
+        <v>5</v>
+      </c>
+      <c r="AY118" s="2">
+        <v>4</v>
+      </c>
+      <c r="AZ118" s="2">
+        <v>6</v>
+      </c>
+      <c r="BA118" s="2">
+        <v>5</v>
+      </c>
+      <c r="BB118" s="2">
+        <v>4</v>
+      </c>
+      <c r="BC118" s="2">
+        <v>5</v>
+      </c>
+      <c r="BD118" s="2">
+        <v>4</v>
+      </c>
+      <c r="BE118" s="2">
+        <v>2</v>
+      </c>
+      <c r="BF118" s="2">
+        <v>3</v>
+      </c>
+      <c r="BG118" s="2">
+        <v>5</v>
+      </c>
+      <c r="BH118" s="2">
+        <v>6</v>
+      </c>
+      <c r="BI118" s="2">
+        <v>7</v>
+      </c>
+      <c r="BJ118" s="2">
+        <v>1</v>
+      </c>
+      <c r="BK118" s="2">
+        <v>4</v>
+      </c>
+      <c r="BL118" s="2">
+        <v>2</v>
+      </c>
+      <c r="BM118" s="2">
+        <v>4</v>
+      </c>
+      <c r="BN118" s="2">
+        <v>2</v>
+      </c>
+      <c r="BO118" s="2">
+        <v>1</v>
+      </c>
+      <c r="BP118" s="2">
+        <v>3</v>
+      </c>
+      <c r="BQ118" s="2">
+        <v>5</v>
+      </c>
+      <c r="BR118" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS118" s="2">
+        <v>5</v>
+      </c>
+      <c r="BT118" s="2">
+        <v>4</v>
+      </c>
+      <c r="BU118" s="2">
+        <v>4</v>
+      </c>
+      <c r="BV118" s="2">
+        <v>5</v>
+      </c>
+      <c r="BW118" s="2">
+        <v>3</v>
+      </c>
+      <c r="BX118" s="2">
+        <v>3</v>
+      </c>
+      <c r="BY118" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ118" s="3">
+        <v>9.6853333333333342</v>
+      </c>
+    </row>
+    <row r="119" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>30</v>
+      </c>
+      <c r="B119" s="2">
+        <v>1</v>
+      </c>
+      <c r="C119" s="2">
+        <v>6</v>
+      </c>
+      <c r="D119" s="2">
+        <v>0</v>
+      </c>
+      <c r="E119" s="2">
+        <v>1</v>
+      </c>
+      <c r="F119" s="2">
+        <v>1</v>
+      </c>
+      <c r="G119" s="2">
+        <v>1</v>
+      </c>
+      <c r="H119" s="2">
+        <v>1</v>
+      </c>
+      <c r="I119" s="2">
+        <v>1</v>
+      </c>
+      <c r="J119" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="K119" s="2">
+        <v>4</v>
+      </c>
+      <c r="L119" s="2">
+        <v>1</v>
+      </c>
+      <c r="M119" s="2">
+        <v>1</v>
+      </c>
+      <c r="N119" s="2">
+        <v>0</v>
+      </c>
+      <c r="O119" s="2">
+        <v>6</v>
+      </c>
+      <c r="P119" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q119" s="2">
+        <v>4</v>
+      </c>
+      <c r="R119" s="2">
+        <v>3</v>
+      </c>
+      <c r="S119" s="2">
+        <v>4</v>
+      </c>
+      <c r="T119" s="2">
+        <v>3</v>
+      </c>
+      <c r="U119" s="2">
+        <v>3</v>
+      </c>
+      <c r="V119" s="2">
+        <v>2</v>
+      </c>
+      <c r="W119" s="2">
+        <v>6</v>
+      </c>
+      <c r="X119" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y119" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z119" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA119" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB119" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC119" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD119" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE119" s="2">
+        <v>2</v>
+      </c>
+      <c r="AF119" s="2">
+        <v>6</v>
+      </c>
+      <c r="AG119" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH119" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI119" s="2">
+        <v>4</v>
+      </c>
+      <c r="AJ119" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK119" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL119" s="2">
+        <v>4</v>
+      </c>
+      <c r="AM119" s="2">
+        <v>6</v>
+      </c>
+      <c r="AN119" s="2">
+        <v>5</v>
+      </c>
+      <c r="AO119" s="2">
+        <v>6</v>
+      </c>
+      <c r="AP119" s="2">
+        <v>7</v>
+      </c>
+      <c r="AQ119" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR119" s="2">
+        <v>6</v>
+      </c>
+      <c r="AS119" s="2">
+        <v>6</v>
+      </c>
+      <c r="AT119" s="2">
+        <v>4</v>
+      </c>
+      <c r="AU119" s="2">
+        <v>5</v>
+      </c>
+      <c r="AV119" s="2">
+        <v>4</v>
+      </c>
+      <c r="AW119" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX119" s="2">
+        <v>6</v>
+      </c>
+      <c r="AY119" s="2">
+        <v>4</v>
+      </c>
+      <c r="AZ119" s="2">
+        <v>7</v>
+      </c>
+      <c r="BA119" s="2">
+        <v>4</v>
+      </c>
+      <c r="BB119" s="2">
+        <v>7</v>
+      </c>
+      <c r="BC119" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD119" s="2">
+        <v>5</v>
+      </c>
+      <c r="BE119" s="2">
+        <v>3</v>
+      </c>
+      <c r="BF119" s="2">
+        <v>1</v>
+      </c>
+      <c r="BG119" s="2">
+        <v>6</v>
+      </c>
+      <c r="BH119" s="2">
+        <v>5</v>
+      </c>
+      <c r="BI119" s="2">
+        <v>7</v>
+      </c>
+      <c r="BJ119" s="2">
+        <v>3</v>
+      </c>
+      <c r="BK119" s="2">
+        <v>4</v>
+      </c>
+      <c r="BL119" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM119" s="2">
+        <v>5</v>
+      </c>
+      <c r="BN119" s="2">
+        <v>5</v>
+      </c>
+      <c r="BO119" s="2">
+        <v>6</v>
+      </c>
+      <c r="BP119" s="2">
+        <v>6</v>
+      </c>
+      <c r="BQ119" s="2">
+        <v>5</v>
+      </c>
+      <c r="BR119" s="2">
+        <v>7</v>
+      </c>
+      <c r="BS119" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT119" s="2">
+        <v>4</v>
+      </c>
+      <c r="BU119" s="2">
+        <v>3</v>
+      </c>
+      <c r="BV119" s="2">
+        <v>4</v>
+      </c>
+      <c r="BW119" s="2">
+        <v>3</v>
+      </c>
+      <c r="BX119" s="2">
+        <v>4</v>
+      </c>
+      <c r="BY119" s="2">
+        <v>5</v>
+      </c>
+      <c r="BZ119" s="3">
+        <v>15.766500000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>22</v>
+      </c>
+      <c r="B120" s="2">
+        <v>2</v>
+      </c>
+      <c r="C120" s="2">
+        <v>4</v>
+      </c>
+      <c r="D120" s="2">
+        <v>3</v>
+      </c>
+      <c r="E120" s="2">
+        <v>1</v>
+      </c>
+      <c r="F120" s="2">
+        <v>3</v>
+      </c>
+      <c r="G120" s="2">
+        <v>1</v>
+      </c>
+      <c r="H120" s="2">
+        <v>1</v>
+      </c>
+      <c r="I120" s="2">
+        <v>2</v>
+      </c>
+      <c r="J120" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K120" s="2">
+        <v>7</v>
+      </c>
+      <c r="L120" s="2">
+        <v>0</v>
+      </c>
+      <c r="M120" s="2">
+        <v>0</v>
+      </c>
+      <c r="N120" s="2">
+        <v>1</v>
+      </c>
+      <c r="O120" s="2">
+        <v>6</v>
+      </c>
+      <c r="P120" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q120" s="2">
+        <v>3</v>
+      </c>
+      <c r="R120" s="2">
+        <v>4</v>
+      </c>
+      <c r="S120" s="2">
+        <v>4</v>
+      </c>
+      <c r="T120" s="2">
+        <v>3</v>
+      </c>
+      <c r="U120" s="2">
+        <v>3</v>
+      </c>
+      <c r="V120" s="2">
+        <v>2</v>
+      </c>
+      <c r="W120" s="2">
+        <v>5</v>
+      </c>
+      <c r="X120" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y120" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z120" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA120" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB120" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC120" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD120" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE120" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF120" s="2">
+        <v>5</v>
+      </c>
+      <c r="AG120" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH120" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI120" s="2">
+        <v>4</v>
+      </c>
+      <c r="AJ120" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK120" s="2">
+        <v>6</v>
+      </c>
+      <c r="AL120" s="2">
+        <v>4</v>
+      </c>
+      <c r="AM120" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN120" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO120" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP120" s="2">
+        <v>6</v>
+      </c>
+      <c r="AQ120" s="2">
+        <v>7</v>
+      </c>
+      <c r="AR120" s="2">
+        <v>7</v>
+      </c>
+      <c r="AS120" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT120" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU120" s="2">
+        <v>6</v>
+      </c>
+      <c r="AV120" s="2">
+        <v>6</v>
+      </c>
+      <c r="AW120" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX120" s="2">
+        <v>6</v>
+      </c>
+      <c r="AY120" s="2">
+        <v>6</v>
+      </c>
+      <c r="AZ120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BA120" s="2">
+        <v>6</v>
+      </c>
+      <c r="BB120" s="2">
+        <v>6</v>
+      </c>
+      <c r="BC120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BD120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BE120" s="2">
+        <v>6</v>
+      </c>
+      <c r="BF120" s="2">
+        <v>7</v>
+      </c>
+      <c r="BG120" s="2">
+        <v>3</v>
+      </c>
+      <c r="BH120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BI120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BJ120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BK120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BL120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BM120" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BO120" s="2">
+        <v>5</v>
+      </c>
+      <c r="BP120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BQ120" s="2">
+        <v>6</v>
+      </c>
+      <c r="BR120" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS120" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT120" s="2">
+        <v>3</v>
+      </c>
+      <c r="BU120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BV120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BW120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BX120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BY120" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ120" s="3">
+        <v>23.423500000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>39</v>
+      </c>
+      <c r="B121" s="2">
+        <v>2</v>
+      </c>
+      <c r="C121" s="2">
+        <v>6</v>
+      </c>
+      <c r="D121" s="2">
+        <v>24</v>
+      </c>
+      <c r="E121" s="2">
+        <v>1</v>
+      </c>
+      <c r="F121" s="2">
+        <v>3</v>
+      </c>
+      <c r="G121" s="2">
+        <v>1</v>
+      </c>
+      <c r="H121" s="2">
+        <v>1</v>
+      </c>
+      <c r="I121" s="2">
+        <v>1</v>
+      </c>
+      <c r="J121" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K121" s="2">
+        <v>0</v>
+      </c>
+      <c r="L121" s="2">
+        <v>0</v>
+      </c>
+      <c r="M121" s="2">
+        <v>1</v>
+      </c>
+      <c r="N121" s="2">
+        <v>0</v>
+      </c>
+      <c r="O121" s="2">
+        <v>6</v>
+      </c>
+      <c r="P121" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q121" s="2">
+        <v>4</v>
+      </c>
+      <c r="R121" s="2">
+        <v>5</v>
+      </c>
+      <c r="S121" s="2">
+        <v>5</v>
+      </c>
+      <c r="T121" s="2">
+        <v>4</v>
+      </c>
+      <c r="U121" s="2">
+        <v>4</v>
+      </c>
+      <c r="V121" s="2">
+        <v>3</v>
+      </c>
+      <c r="W121" s="2">
+        <v>7</v>
+      </c>
+      <c r="X121" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y121" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AA121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AB121" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC121" s="2">
+        <v>5</v>
+      </c>
+      <c r="AD121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF121" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AH121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AL121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AM121" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN121" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO121" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AQ121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AS121" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AV121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AW121" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AY121" s="2">
+        <v>6</v>
+      </c>
+      <c r="AZ121" s="2">
+        <v>7</v>
+      </c>
+      <c r="BA121" s="2">
+        <v>7</v>
+      </c>
+      <c r="BB121" s="2">
+        <v>7</v>
+      </c>
+      <c r="BC121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD121" s="2">
+        <v>7</v>
+      </c>
+      <c r="BE121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BF121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BG121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BH121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BI121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BJ121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BK121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BL121" s="2">
+        <v>3</v>
+      </c>
+      <c r="BM121" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BO121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BP121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BQ121" s="2">
+        <v>7</v>
+      </c>
+      <c r="BR121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS121" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BU121" s="2">
+        <v>3</v>
+      </c>
+      <c r="BV121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BW121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BX121" s="2">
+        <v>5</v>
+      </c>
+      <c r="BY121" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ121" s="3">
+        <v>16.439499999999999</v>
+      </c>
+    </row>
+    <row r="122" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>27</v>
+      </c>
+      <c r="B122" s="2">
+        <v>2</v>
+      </c>
+      <c r="C122" s="2">
+        <v>6</v>
+      </c>
+      <c r="D122" s="2">
+        <v>9</v>
+      </c>
+      <c r="E122" s="2">
+        <v>1</v>
+      </c>
+      <c r="F122" s="2">
+        <v>3</v>
+      </c>
+      <c r="G122" s="2">
+        <v>4</v>
+      </c>
+      <c r="H122" s="2">
+        <v>1</v>
+      </c>
+      <c r="I122" s="2">
+        <v>1</v>
+      </c>
+      <c r="J122" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K122" s="2">
+        <v>2</v>
+      </c>
+      <c r="L122" s="2">
+        <v>1</v>
+      </c>
+      <c r="M122" s="2">
+        <v>1</v>
+      </c>
+      <c r="N122" s="2">
+        <v>0</v>
+      </c>
+      <c r="O122" s="2">
+        <v>6</v>
+      </c>
+      <c r="P122" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q122" s="2">
+        <v>6</v>
+      </c>
+      <c r="R122" s="2">
+        <v>6</v>
+      </c>
+      <c r="S122" s="2">
+        <v>6</v>
+      </c>
+      <c r="T122" s="2">
+        <v>3</v>
+      </c>
+      <c r="U122" s="2">
+        <v>5</v>
+      </c>
+      <c r="V122" s="2">
+        <v>5</v>
+      </c>
+      <c r="W122" s="2">
+        <v>7</v>
+      </c>
+      <c r="X122" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y122" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z122" s="2">
+        <v>5</v>
+      </c>
+      <c r="AA122" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AC122" s="2">
+        <v>4</v>
+      </c>
+      <c r="AD122" s="2">
+        <v>3</v>
+      </c>
+      <c r="AE122" s="2">
+        <v>4</v>
+      </c>
+      <c r="AF122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AH122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ122" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AL122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AM122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AP122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AQ122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AS122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AV122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AW122" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX122" s="2">
+        <v>6</v>
+      </c>
+      <c r="AY122" s="2">
+        <v>7</v>
+      </c>
+      <c r="AZ122" s="2">
+        <v>6</v>
+      </c>
+      <c r="BA122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BB122" s="2">
+        <v>7</v>
+      </c>
+      <c r="BC122" s="2">
+        <v>7</v>
+      </c>
+      <c r="BD122" s="2">
+        <v>7</v>
+      </c>
+      <c r="BE122" s="2">
+        <v>2</v>
+      </c>
+      <c r="BF122" s="2">
+        <v>4</v>
+      </c>
+      <c r="BG122" s="2">
+        <v>3</v>
+      </c>
+      <c r="BH122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BI122" s="2">
+        <v>7</v>
+      </c>
+      <c r="BJ122" s="2">
+        <v>7</v>
+      </c>
+      <c r="BK122" s="2">
+        <v>3</v>
+      </c>
+      <c r="BL122" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM122" s="2">
+        <v>4</v>
+      </c>
+      <c r="BN122" s="2">
+        <v>4</v>
+      </c>
+      <c r="BO122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BP122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BQ122" s="2">
+        <v>7</v>
+      </c>
+      <c r="BR122" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS122" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT122" s="2">
+        <v>3</v>
+      </c>
+      <c r="BU122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BV122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BW122" s="2">
+        <v>4</v>
+      </c>
+      <c r="BX122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BY122" s="2">
+        <v>5</v>
+      </c>
+      <c r="BZ122" s="3">
+        <v>13.94</v>
+      </c>
+    </row>
+    <row r="123" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>31</v>
+      </c>
+      <c r="B123" s="2">
+        <v>2</v>
+      </c>
+      <c r="C123" s="2">
+        <v>6</v>
+      </c>
+      <c r="D123" s="2">
+        <v>6</v>
+      </c>
+      <c r="E123" s="2">
+        <v>1</v>
+      </c>
+      <c r="F123" s="2">
+        <v>3</v>
+      </c>
+      <c r="G123" s="2">
+        <v>2</v>
+      </c>
+      <c r="H123" s="2">
+        <v>1</v>
+      </c>
+      <c r="I123" s="2">
+        <v>2</v>
+      </c>
+      <c r="J123" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K123" s="2">
+        <v>6</v>
+      </c>
+      <c r="L123" s="2">
+        <v>1</v>
+      </c>
+      <c r="M123" s="2">
+        <v>1</v>
+      </c>
+      <c r="N123" s="2">
+        <v>0</v>
+      </c>
+      <c r="O123" s="2">
+        <v>6</v>
+      </c>
+      <c r="P123" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q123" s="2">
+        <v>5</v>
+      </c>
+      <c r="R123" s="2">
+        <v>6</v>
+      </c>
+      <c r="S123" s="2">
+        <v>7</v>
+      </c>
+      <c r="T123" s="2">
+        <v>1</v>
+      </c>
+      <c r="U123" s="2">
+        <v>1</v>
+      </c>
+      <c r="V123" s="2">
+        <v>5</v>
+      </c>
+      <c r="W123" s="2">
+        <v>7</v>
+      </c>
+      <c r="X123" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y123" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z123" s="2">
+        <v>3</v>
+      </c>
+      <c r="AA123" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AC123" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD123" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE123" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AH123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AI123" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ123" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AL123" s="2">
+        <v>4</v>
+      </c>
+      <c r="AM123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO123" s="2">
+        <v>4</v>
+      </c>
+      <c r="AP123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AQ123" s="2">
+        <v>1</v>
+      </c>
+      <c r="AR123" s="2">
+        <v>4</v>
+      </c>
+      <c r="AS123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AT123" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AV123" s="2">
+        <v>7</v>
+      </c>
+      <c r="AW123" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX123" s="2">
+        <v>5</v>
+      </c>
+      <c r="AY123" s="2">
+        <v>6</v>
+      </c>
+      <c r="AZ123" s="2">
+        <v>7</v>
+      </c>
+      <c r="BA123" s="2">
+        <v>6</v>
+      </c>
+      <c r="BB123" s="2">
+        <v>7</v>
+      </c>
+      <c r="BC123" s="2">
+        <v>6</v>
+      </c>
+      <c r="BD123" s="2">
+        <v>2</v>
+      </c>
+      <c r="BE123" s="2">
+        <v>4</v>
+      </c>
+      <c r="BF123" s="2">
+        <v>3</v>
+      </c>
+      <c r="BG123" s="2">
+        <v>2</v>
+      </c>
+      <c r="BH123" s="2">
+        <v>6</v>
+      </c>
+      <c r="BI123" s="2">
+        <v>7</v>
+      </c>
+      <c r="BJ123" s="2">
+        <v>4</v>
+      </c>
+      <c r="BK123" s="2">
+        <v>4</v>
+      </c>
+      <c r="BL123" s="2">
+        <v>1</v>
+      </c>
+      <c r="BM123" s="2">
+        <v>2</v>
+      </c>
+      <c r="BN123" s="2">
+        <v>2</v>
+      </c>
+      <c r="BO123" s="2">
+        <v>4</v>
+      </c>
+      <c r="BP123" s="2">
+        <v>1</v>
+      </c>
+      <c r="BQ123" s="2">
+        <v>7</v>
+      </c>
+      <c r="BR123" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS123" s="2">
+        <v>7</v>
+      </c>
+      <c r="BT123" s="2">
+        <v>3</v>
+      </c>
+      <c r="BU123" s="2">
+        <v>3</v>
+      </c>
+      <c r="BV123" s="2">
+        <v>5</v>
+      </c>
+      <c r="BW123" s="2">
+        <v>3</v>
+      </c>
+      <c r="BX123" s="2">
+        <v>5</v>
+      </c>
+      <c r="BY123" s="2">
+        <v>5</v>
+      </c>
+      <c r="BZ123" s="3">
+        <v>26.33966666666667</v>
+      </c>
+    </row>
+    <row r="124" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>35</v>
+      </c>
+      <c r="B124" s="2">
+        <v>2</v>
+      </c>
+      <c r="C124" s="2">
+        <v>6</v>
+      </c>
+      <c r="D124" s="2">
+        <v>9</v>
+      </c>
+      <c r="E124" s="2">
+        <v>1</v>
+      </c>
+      <c r="F124" s="2">
+        <v>1</v>
+      </c>
+      <c r="G124" s="2">
+        <v>4</v>
+      </c>
+      <c r="H124" s="2">
+        <v>1</v>
+      </c>
+      <c r="I124" s="2">
+        <v>1</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K124" s="2">
+        <v>9</v>
+      </c>
+      <c r="L124" s="2">
+        <v>1</v>
+      </c>
+      <c r="M124" s="2">
+        <v>0</v>
+      </c>
+      <c r="N124" s="2">
+        <v>1</v>
+      </c>
+      <c r="O124" s="2">
+        <v>6</v>
+      </c>
+      <c r="P124" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q124" s="2">
+        <v>5</v>
+      </c>
+      <c r="R124" s="2">
+        <v>6</v>
+      </c>
+      <c r="S124" s="2">
+        <v>7</v>
+      </c>
+      <c r="T124" s="2">
+        <v>3</v>
+      </c>
+      <c r="U124" s="2">
+        <v>4</v>
+      </c>
+      <c r="V124" s="2">
+        <v>5</v>
+      </c>
+      <c r="W124" s="2">
+        <v>7</v>
+      </c>
+      <c r="X124" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y124" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z124" s="2">
+        <v>5</v>
+      </c>
+      <c r="AA124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AB124" s="2">
+        <v>7</v>
+      </c>
+      <c r="AC124" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD124" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AF124" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG124" s="2">
+        <v>7</v>
+      </c>
+      <c r="AH124" s="2">
+        <v>5</v>
+      </c>
+      <c r="AI124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AJ124" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK124" s="2">
+        <v>5</v>
+      </c>
+      <c r="AL124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AM124" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AO124" s="2">
+        <v>5</v>
+      </c>
+      <c r="AP124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AQ124" s="2">
+        <v>7</v>
+      </c>
+      <c r="AR124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AS124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AT124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AU124" s="2">
+        <v>5</v>
+      </c>
+      <c r="AV124" s="2">
+        <v>7</v>
+      </c>
+      <c r="AW124" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX124" s="2">
+        <v>7</v>
+      </c>
+      <c r="AY124" s="2">
+        <v>6</v>
+      </c>
+      <c r="AZ124" s="2">
+        <v>5</v>
+      </c>
+      <c r="BA124" s="2">
+        <v>7</v>
+      </c>
+      <c r="BB124" s="2">
+        <v>5</v>
+      </c>
+      <c r="BC124" s="2">
+        <v>7</v>
+      </c>
+      <c r="BD124" s="2">
+        <v>6</v>
+      </c>
+      <c r="BE124" s="2">
+        <v>5</v>
+      </c>
+      <c r="BF124" s="2">
+        <v>6</v>
+      </c>
+      <c r="BG124" s="2">
+        <v>2</v>
+      </c>
+      <c r="BH124" s="2">
+        <v>2</v>
+      </c>
+      <c r="BI124" s="2">
+        <v>3</v>
+      </c>
+      <c r="BJ124" s="2">
+        <v>5</v>
+      </c>
+      <c r="BK124" s="2">
+        <v>6</v>
+      </c>
+      <c r="BL124" s="2">
+        <v>6</v>
+      </c>
+      <c r="BM124" s="2">
+        <v>3</v>
+      </c>
+      <c r="BN124" s="2">
+        <v>3</v>
+      </c>
+      <c r="BO124" s="2">
+        <v>5</v>
+      </c>
+      <c r="BP124" s="2">
+        <v>4</v>
+      </c>
+      <c r="BQ124" s="2">
+        <v>7</v>
+      </c>
+      <c r="BR124" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS124" s="2">
+        <v>7</v>
+      </c>
+      <c r="BT124" s="2">
+        <v>5</v>
+      </c>
+      <c r="BU124" s="2">
+        <v>4</v>
+      </c>
+      <c r="BV124" s="2">
+        <v>4</v>
+      </c>
+      <c r="BW124" s="2">
+        <v>4</v>
+      </c>
+      <c r="BX124" s="2">
+        <v>5</v>
+      </c>
+      <c r="BY124" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ124" s="3">
+        <v>10.832833333333333</v>
+      </c>
+    </row>
+    <row r="125" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>32</v>
+      </c>
+      <c r="B125" s="2">
+        <v>2</v>
+      </c>
+      <c r="C125" s="2">
+        <v>6</v>
+      </c>
+      <c r="D125" s="2">
+        <v>7</v>
+      </c>
+      <c r="E125" s="2">
+        <v>1</v>
+      </c>
+      <c r="F125" s="2">
+        <v>1</v>
+      </c>
+      <c r="G125" s="2">
+        <v>4</v>
+      </c>
+      <c r="H125" s="2">
+        <v>1</v>
+      </c>
+      <c r="I125" s="2">
+        <v>1</v>
+      </c>
+      <c r="J125" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K125" s="2">
+        <v>12</v>
+      </c>
+      <c r="L125" s="2">
+        <v>1</v>
+      </c>
+      <c r="M125" s="2">
+        <v>1</v>
+      </c>
+      <c r="N125" s="2">
+        <v>1</v>
+      </c>
+      <c r="O125" s="2">
+        <v>6</v>
+      </c>
+      <c r="P125" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q125" s="2">
+        <v>3</v>
+      </c>
+      <c r="R125" s="2">
+        <v>5</v>
+      </c>
+      <c r="S125" s="2">
+        <v>1</v>
+      </c>
+      <c r="T125" s="2">
+        <v>3</v>
+      </c>
+      <c r="U125" s="2">
+        <v>7</v>
+      </c>
+      <c r="V125" s="2">
+        <v>7</v>
+      </c>
+      <c r="W125" s="2">
+        <v>6</v>
+      </c>
+      <c r="X125" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y125" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z125" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA125" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB125" s="2">
+        <v>5</v>
+      </c>
+      <c r="AC125" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD125" s="2">
+        <v>4</v>
+      </c>
+      <c r="AE125" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AG125" s="2">
+        <v>6</v>
+      </c>
+      <c r="AH125" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI125" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ125" s="2">
+        <v>4</v>
+      </c>
+      <c r="AK125" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL125" s="2">
+        <v>2</v>
+      </c>
+      <c r="AM125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AN125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AO125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AP125" s="2">
+        <v>6</v>
+      </c>
+      <c r="AQ125" s="2">
+        <v>6</v>
+      </c>
+      <c r="AR125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AS125" s="2">
+        <v>5</v>
+      </c>
+      <c r="AT125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AU125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AV125" s="2">
+        <v>7</v>
+      </c>
+      <c r="AW125" s="2">
+        <v>4</v>
+      </c>
+      <c r="AX125" s="2">
+        <v>5</v>
+      </c>
+      <c r="AY125" s="2">
+        <v>6</v>
+      </c>
+      <c r="AZ125" s="2">
+        <v>6</v>
+      </c>
+      <c r="BA125" s="2">
+        <v>6</v>
+      </c>
+      <c r="BB125" s="2">
+        <v>6</v>
+      </c>
+      <c r="BC125" s="2">
+        <v>7</v>
+      </c>
+      <c r="BD125" s="2">
+        <v>6</v>
+      </c>
+      <c r="BE125" s="2">
+        <v>5</v>
+      </c>
+      <c r="BF125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BG125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BH125" s="2">
+        <v>5</v>
+      </c>
+      <c r="BI125" s="2">
+        <v>3</v>
+      </c>
+      <c r="BJ125" s="2">
+        <v>2</v>
+      </c>
+      <c r="BK125" s="2">
+        <v>6</v>
+      </c>
+      <c r="BL125" s="2">
+        <v>2</v>
+      </c>
+      <c r="BM125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BN125" s="2">
+        <v>3</v>
+      </c>
+      <c r="BO125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BP125" s="2">
+        <v>5</v>
+      </c>
+      <c r="BQ125" s="2">
+        <v>7</v>
+      </c>
+      <c r="BR125" s="2">
+        <v>6</v>
+      </c>
+      <c r="BS125" s="2">
+        <v>6</v>
+      </c>
+      <c r="BT125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BU125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BV125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BW125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BX125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BY125" s="2">
+        <v>4</v>
+      </c>
+      <c r="BZ125" s="3">
+        <v>10.610666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Updating manual data - Multilevel modelling (different cases)
</commit_message>
<xml_diff>
--- a/Data_EE Downward Causation_Conjoint_Wave3.xlsx
+++ b/Data_EE Downward Causation_Conjoint_Wave3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johannes.haehnlein\Desktop\Johannes Haehnlein\19_PROMOTION\01_STUDIEN\Studie 2 - Conjoint\Data\R Repository\EE_Downward-Causation_Entrepreneurship-Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F109BAC4-DE22-4302-8BEF-61B94645690E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE1664E-21A4-4857-85F8-212783D60615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Studie zur Stärkung von Gründun" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="139">
   <si>
     <t>age</t>
   </si>
@@ -446,19 +446,10 @@
     <t>duration</t>
   </si>
   <si>
-    <t>Ludwigshafen</t>
-  </si>
-  <si>
     <t>Hofheim</t>
   </si>
   <si>
     <t>Kassel</t>
-  </si>
-  <si>
-    <t>Köln</t>
-  </si>
-  <si>
-    <t>Göttingen</t>
   </si>
 </sst>
 </file>
@@ -493,11 +484,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -812,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ125"/>
+  <dimension ref="A1:BZ114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120:XFD125"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7227,7 +7217,7 @@
         <v>9</v>
       </c>
       <c r="J28" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -22782,7 +22772,7 @@
         <v>7</v>
       </c>
       <c r="J94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K94">
         <v>50</v>
@@ -27698,2602 +27688,6 @@
       </c>
       <c r="BZ114" s="1">
         <v>11.932666666666668</v>
-      </c>
-    </row>
-    <row r="115" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A115">
-        <v>42</v>
-      </c>
-      <c r="B115">
-        <v>2</v>
-      </c>
-      <c r="C115">
-        <v>6</v>
-      </c>
-      <c r="D115">
-        <v>25</v>
-      </c>
-      <c r="E115">
-        <v>1</v>
-      </c>
-      <c r="F115">
-        <v>2</v>
-      </c>
-      <c r="G115">
-        <v>6</v>
-      </c>
-      <c r="H115">
-        <v>1</v>
-      </c>
-      <c r="I115">
-        <v>1</v>
-      </c>
-      <c r="J115" t="s">
-        <v>41</v>
-      </c>
-      <c r="K115">
-        <v>6</v>
-      </c>
-      <c r="L115">
-        <v>1</v>
-      </c>
-      <c r="M115">
-        <v>1</v>
-      </c>
-      <c r="N115">
-        <v>0</v>
-      </c>
-      <c r="O115">
-        <v>6</v>
-      </c>
-      <c r="P115">
-        <v>2</v>
-      </c>
-      <c r="Q115">
-        <v>2</v>
-      </c>
-      <c r="R115">
-        <v>2</v>
-      </c>
-      <c r="S115">
-        <v>7</v>
-      </c>
-      <c r="T115">
-        <v>3</v>
-      </c>
-      <c r="U115">
-        <v>2</v>
-      </c>
-      <c r="V115">
-        <v>2</v>
-      </c>
-      <c r="W115">
-        <v>7</v>
-      </c>
-      <c r="X115">
-        <v>4</v>
-      </c>
-      <c r="Y115">
-        <v>2</v>
-      </c>
-      <c r="Z115">
-        <v>2</v>
-      </c>
-      <c r="AA115">
-        <v>2</v>
-      </c>
-      <c r="AB115">
-        <v>7</v>
-      </c>
-      <c r="AC115">
-        <v>2</v>
-      </c>
-      <c r="AD115">
-        <v>2</v>
-      </c>
-      <c r="AE115">
-        <v>2</v>
-      </c>
-      <c r="AF115">
-        <v>7</v>
-      </c>
-      <c r="AG115">
-        <v>5</v>
-      </c>
-      <c r="AH115">
-        <v>5</v>
-      </c>
-      <c r="AI115">
-        <v>5</v>
-      </c>
-      <c r="AJ115">
-        <v>4</v>
-      </c>
-      <c r="AK115">
-        <v>5</v>
-      </c>
-      <c r="AL115">
-        <v>3</v>
-      </c>
-      <c r="AM115">
-        <v>6</v>
-      </c>
-      <c r="AN115">
-        <v>7</v>
-      </c>
-      <c r="AO115">
-        <v>7</v>
-      </c>
-      <c r="AP115">
-        <v>6</v>
-      </c>
-      <c r="AQ115">
-        <v>6</v>
-      </c>
-      <c r="AR115">
-        <v>6</v>
-      </c>
-      <c r="AS115">
-        <v>6</v>
-      </c>
-      <c r="AT115">
-        <v>6</v>
-      </c>
-      <c r="AU115">
-        <v>7</v>
-      </c>
-      <c r="AV115">
-        <v>5</v>
-      </c>
-      <c r="AW115">
-        <v>4</v>
-      </c>
-      <c r="AX115">
-        <v>6</v>
-      </c>
-      <c r="AY115">
-        <v>6</v>
-      </c>
-      <c r="AZ115">
-        <v>7</v>
-      </c>
-      <c r="BA115">
-        <v>6</v>
-      </c>
-      <c r="BB115">
-        <v>6</v>
-      </c>
-      <c r="BC115">
-        <v>6</v>
-      </c>
-      <c r="BD115">
-        <v>5</v>
-      </c>
-      <c r="BE115">
-        <v>4</v>
-      </c>
-      <c r="BF115">
-        <v>4</v>
-      </c>
-      <c r="BG115">
-        <v>4</v>
-      </c>
-      <c r="BH115">
-        <v>4</v>
-      </c>
-      <c r="BI115">
-        <v>7</v>
-      </c>
-      <c r="BJ115">
-        <v>1</v>
-      </c>
-      <c r="BK115">
-        <v>4</v>
-      </c>
-      <c r="BL115">
-        <v>1</v>
-      </c>
-      <c r="BM115">
-        <v>4</v>
-      </c>
-      <c r="BN115">
-        <v>4</v>
-      </c>
-      <c r="BO115">
-        <v>4</v>
-      </c>
-      <c r="BP115">
-        <v>4</v>
-      </c>
-      <c r="BQ115">
-        <v>7</v>
-      </c>
-      <c r="BR115">
-        <v>7</v>
-      </c>
-      <c r="BS115">
-        <v>7</v>
-      </c>
-      <c r="BT115">
-        <v>5</v>
-      </c>
-      <c r="BU115">
-        <v>5</v>
-      </c>
-      <c r="BV115">
-        <v>5</v>
-      </c>
-      <c r="BW115">
-        <v>5</v>
-      </c>
-      <c r="BX115">
-        <v>5</v>
-      </c>
-      <c r="BY115">
-        <v>5</v>
-      </c>
-      <c r="BZ115" s="1">
-        <v>11.556666666666667</v>
-      </c>
-    </row>
-    <row r="116" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>35</v>
-      </c>
-      <c r="B116">
-        <v>2</v>
-      </c>
-      <c r="C116">
-        <v>7</v>
-      </c>
-      <c r="D116">
-        <v>9</v>
-      </c>
-      <c r="E116">
-        <v>1</v>
-      </c>
-      <c r="F116">
-        <v>1</v>
-      </c>
-      <c r="G116">
-        <v>5</v>
-      </c>
-      <c r="H116">
-        <v>1</v>
-      </c>
-      <c r="I116">
-        <v>2</v>
-      </c>
-      <c r="J116" t="s">
-        <v>46</v>
-      </c>
-      <c r="K116">
-        <v>5</v>
-      </c>
-      <c r="L116">
-        <v>0</v>
-      </c>
-      <c r="M116">
-        <v>0</v>
-      </c>
-      <c r="N116">
-        <v>0</v>
-      </c>
-      <c r="O116">
-        <v>6</v>
-      </c>
-      <c r="P116">
-        <v>4</v>
-      </c>
-      <c r="Q116">
-        <v>6</v>
-      </c>
-      <c r="R116">
-        <v>5</v>
-      </c>
-      <c r="S116">
-        <v>6</v>
-      </c>
-      <c r="T116">
-        <v>2</v>
-      </c>
-      <c r="U116">
-        <v>5</v>
-      </c>
-      <c r="V116">
-        <v>4</v>
-      </c>
-      <c r="W116">
-        <v>7</v>
-      </c>
-      <c r="X116">
-        <v>4</v>
-      </c>
-      <c r="Y116">
-        <v>5</v>
-      </c>
-      <c r="Z116">
-        <v>5</v>
-      </c>
-      <c r="AA116">
-        <v>4</v>
-      </c>
-      <c r="AB116">
-        <v>6</v>
-      </c>
-      <c r="AC116">
-        <v>4</v>
-      </c>
-      <c r="AD116">
-        <v>5</v>
-      </c>
-      <c r="AE116">
-        <v>4</v>
-      </c>
-      <c r="AF116">
-        <v>7</v>
-      </c>
-      <c r="AG116">
-        <v>1</v>
-      </c>
-      <c r="AH116">
-        <v>5</v>
-      </c>
-      <c r="AI116">
-        <v>5</v>
-      </c>
-      <c r="AJ116">
-        <v>4</v>
-      </c>
-      <c r="AK116">
-        <v>6</v>
-      </c>
-      <c r="AL116">
-        <v>5</v>
-      </c>
-      <c r="AM116">
-        <v>7</v>
-      </c>
-      <c r="AN116">
-        <v>7</v>
-      </c>
-      <c r="AO116">
-        <v>7</v>
-      </c>
-      <c r="AP116">
-        <v>5</v>
-      </c>
-      <c r="AQ116">
-        <v>4</v>
-      </c>
-      <c r="AR116">
-        <v>4</v>
-      </c>
-      <c r="AS116">
-        <v>5</v>
-      </c>
-      <c r="AT116">
-        <v>7</v>
-      </c>
-      <c r="AU116">
-        <v>4</v>
-      </c>
-      <c r="AV116">
-        <v>7</v>
-      </c>
-      <c r="AW116">
-        <v>4</v>
-      </c>
-      <c r="AX116">
-        <v>5</v>
-      </c>
-      <c r="AY116">
-        <v>5</v>
-      </c>
-      <c r="AZ116">
-        <v>6</v>
-      </c>
-      <c r="BA116">
-        <v>7</v>
-      </c>
-      <c r="BB116">
-        <v>6</v>
-      </c>
-      <c r="BC116">
-        <v>2</v>
-      </c>
-      <c r="BD116">
-        <v>2</v>
-      </c>
-      <c r="BE116">
-        <v>2</v>
-      </c>
-      <c r="BF116">
-        <v>4</v>
-      </c>
-      <c r="BG116">
-        <v>4</v>
-      </c>
-      <c r="BH116">
-        <v>4</v>
-      </c>
-      <c r="BI116">
-        <v>7</v>
-      </c>
-      <c r="BJ116">
-        <v>4</v>
-      </c>
-      <c r="BK116">
-        <v>6</v>
-      </c>
-      <c r="BL116">
-        <v>2</v>
-      </c>
-      <c r="BM116">
-        <v>4</v>
-      </c>
-      <c r="BN116">
-        <v>4</v>
-      </c>
-      <c r="BO116">
-        <v>6</v>
-      </c>
-      <c r="BP116">
-        <v>6</v>
-      </c>
-      <c r="BQ116">
-        <v>7</v>
-      </c>
-      <c r="BR116">
-        <v>7</v>
-      </c>
-      <c r="BS116">
-        <v>6</v>
-      </c>
-      <c r="BT116">
-        <v>2</v>
-      </c>
-      <c r="BU116">
-        <v>3</v>
-      </c>
-      <c r="BV116">
-        <v>3</v>
-      </c>
-      <c r="BW116">
-        <v>2</v>
-      </c>
-      <c r="BX116">
-        <v>4</v>
-      </c>
-      <c r="BY116">
-        <v>4</v>
-      </c>
-      <c r="BZ116" s="1">
-        <v>20.139833333333335</v>
-      </c>
-    </row>
-    <row r="117" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
-        <v>24</v>
-      </c>
-      <c r="B117" s="2">
-        <v>2</v>
-      </c>
-      <c r="C117" s="2">
-        <v>6</v>
-      </c>
-      <c r="D117" s="2">
-        <v>2</v>
-      </c>
-      <c r="E117" s="2">
-        <v>1</v>
-      </c>
-      <c r="F117" s="2">
-        <v>1</v>
-      </c>
-      <c r="G117" s="2">
-        <v>2</v>
-      </c>
-      <c r="H117" s="2">
-        <v>1</v>
-      </c>
-      <c r="I117" s="2">
-        <v>1</v>
-      </c>
-      <c r="J117" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="K117" s="2">
-        <v>0</v>
-      </c>
-      <c r="L117" s="2">
-        <v>0</v>
-      </c>
-      <c r="M117" s="2">
-        <v>1</v>
-      </c>
-      <c r="N117" s="2">
-        <v>0</v>
-      </c>
-      <c r="O117" s="2">
-        <v>6</v>
-      </c>
-      <c r="P117" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q117" s="2">
-        <v>4</v>
-      </c>
-      <c r="R117" s="2">
-        <v>5</v>
-      </c>
-      <c r="S117" s="2">
-        <v>5</v>
-      </c>
-      <c r="T117" s="2">
-        <v>4</v>
-      </c>
-      <c r="U117" s="2">
-        <v>6</v>
-      </c>
-      <c r="V117" s="2">
-        <v>3</v>
-      </c>
-      <c r="W117" s="2">
-        <v>7</v>
-      </c>
-      <c r="X117" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y117" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z117" s="2">
-        <v>4</v>
-      </c>
-      <c r="AA117" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB117" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC117" s="2">
-        <v>4</v>
-      </c>
-      <c r="AD117" s="2">
-        <v>6</v>
-      </c>
-      <c r="AE117" s="2">
-        <v>3</v>
-      </c>
-      <c r="AF117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AG117" s="2">
-        <v>4</v>
-      </c>
-      <c r="AH117" s="2">
-        <v>4</v>
-      </c>
-      <c r="AI117" s="2">
-        <v>2</v>
-      </c>
-      <c r="AJ117" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK117" s="2">
-        <v>5</v>
-      </c>
-      <c r="AL117" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AO117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AP117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AQ117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AR117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AS117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AT117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AU117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AV117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AW117" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AY117" s="2">
-        <v>7</v>
-      </c>
-      <c r="AZ117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BA117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BB117" s="2">
-        <v>6</v>
-      </c>
-      <c r="BC117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BD117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BE117" s="2">
-        <v>5</v>
-      </c>
-      <c r="BF117" s="2">
-        <v>5</v>
-      </c>
-      <c r="BG117" s="2">
-        <v>4</v>
-      </c>
-      <c r="BH117" s="2">
-        <v>6</v>
-      </c>
-      <c r="BI117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BJ117" s="2">
-        <v>6</v>
-      </c>
-      <c r="BK117" s="2">
-        <v>6</v>
-      </c>
-      <c r="BL117" s="2">
-        <v>4</v>
-      </c>
-      <c r="BM117" s="2">
-        <v>3</v>
-      </c>
-      <c r="BN117" s="2">
-        <v>4</v>
-      </c>
-      <c r="BO117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BP117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BQ117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BR117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BS117" s="2">
-        <v>7</v>
-      </c>
-      <c r="BT117" s="2">
-        <v>4</v>
-      </c>
-      <c r="BU117" s="2">
-        <v>4</v>
-      </c>
-      <c r="BV117" s="2">
-        <v>5</v>
-      </c>
-      <c r="BW117" s="2">
-        <v>3</v>
-      </c>
-      <c r="BX117" s="2">
-        <v>4</v>
-      </c>
-      <c r="BY117" s="2">
-        <v>4</v>
-      </c>
-      <c r="BZ117" s="3">
-        <v>9.815666666666667</v>
-      </c>
-    </row>
-    <row r="118" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
-        <v>35</v>
-      </c>
-      <c r="B118" s="2">
-        <v>2</v>
-      </c>
-      <c r="C118" s="2">
-        <v>6</v>
-      </c>
-      <c r="D118" s="2">
-        <v>9</v>
-      </c>
-      <c r="E118" s="2">
-        <v>1</v>
-      </c>
-      <c r="F118" s="2">
-        <v>1</v>
-      </c>
-      <c r="G118" s="2">
-        <v>3</v>
-      </c>
-      <c r="H118" s="2">
-        <v>1</v>
-      </c>
-      <c r="I118" s="2">
-        <v>3</v>
-      </c>
-      <c r="J118" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K118" s="2">
-        <v>23</v>
-      </c>
-      <c r="L118" s="2">
-        <v>1</v>
-      </c>
-      <c r="M118" s="2">
-        <v>1</v>
-      </c>
-      <c r="N118" s="2">
-        <v>0</v>
-      </c>
-      <c r="O118" s="2">
-        <v>6</v>
-      </c>
-      <c r="P118" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q118" s="2">
-        <v>3</v>
-      </c>
-      <c r="R118" s="2">
-        <v>5</v>
-      </c>
-      <c r="S118" s="2">
-        <v>6</v>
-      </c>
-      <c r="T118" s="2">
-        <v>4</v>
-      </c>
-      <c r="U118" s="2">
-        <v>2</v>
-      </c>
-      <c r="V118" s="2">
-        <v>2</v>
-      </c>
-      <c r="W118" s="2">
-        <v>6</v>
-      </c>
-      <c r="X118" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y118" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z118" s="2">
-        <v>2</v>
-      </c>
-      <c r="AA118" s="2">
-        <v>2</v>
-      </c>
-      <c r="AB118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AD118" s="2">
-        <v>4</v>
-      </c>
-      <c r="AE118" s="2">
-        <v>2</v>
-      </c>
-      <c r="AF118" s="2">
-        <v>7</v>
-      </c>
-      <c r="AG118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AH118" s="2">
-        <v>6</v>
-      </c>
-      <c r="AI118" s="2">
-        <v>3</v>
-      </c>
-      <c r="AJ118" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AL118" s="2">
-        <v>2</v>
-      </c>
-      <c r="AM118" s="2">
-        <v>6</v>
-      </c>
-      <c r="AN118" s="2">
-        <v>7</v>
-      </c>
-      <c r="AO118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AP118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AQ118" s="2">
-        <v>6</v>
-      </c>
-      <c r="AR118" s="2">
-        <v>3</v>
-      </c>
-      <c r="AS118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AT118" s="2">
-        <v>3</v>
-      </c>
-      <c r="AU118" s="2">
-        <v>6</v>
-      </c>
-      <c r="AV118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AW118" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX118" s="2">
-        <v>5</v>
-      </c>
-      <c r="AY118" s="2">
-        <v>4</v>
-      </c>
-      <c r="AZ118" s="2">
-        <v>6</v>
-      </c>
-      <c r="BA118" s="2">
-        <v>5</v>
-      </c>
-      <c r="BB118" s="2">
-        <v>4</v>
-      </c>
-      <c r="BC118" s="2">
-        <v>5</v>
-      </c>
-      <c r="BD118" s="2">
-        <v>4</v>
-      </c>
-      <c r="BE118" s="2">
-        <v>2</v>
-      </c>
-      <c r="BF118" s="2">
-        <v>3</v>
-      </c>
-      <c r="BG118" s="2">
-        <v>5</v>
-      </c>
-      <c r="BH118" s="2">
-        <v>6</v>
-      </c>
-      <c r="BI118" s="2">
-        <v>7</v>
-      </c>
-      <c r="BJ118" s="2">
-        <v>1</v>
-      </c>
-      <c r="BK118" s="2">
-        <v>4</v>
-      </c>
-      <c r="BL118" s="2">
-        <v>2</v>
-      </c>
-      <c r="BM118" s="2">
-        <v>4</v>
-      </c>
-      <c r="BN118" s="2">
-        <v>2</v>
-      </c>
-      <c r="BO118" s="2">
-        <v>1</v>
-      </c>
-      <c r="BP118" s="2">
-        <v>3</v>
-      </c>
-      <c r="BQ118" s="2">
-        <v>5</v>
-      </c>
-      <c r="BR118" s="2">
-        <v>6</v>
-      </c>
-      <c r="BS118" s="2">
-        <v>5</v>
-      </c>
-      <c r="BT118" s="2">
-        <v>4</v>
-      </c>
-      <c r="BU118" s="2">
-        <v>4</v>
-      </c>
-      <c r="BV118" s="2">
-        <v>5</v>
-      </c>
-      <c r="BW118" s="2">
-        <v>3</v>
-      </c>
-      <c r="BX118" s="2">
-        <v>3</v>
-      </c>
-      <c r="BY118" s="2">
-        <v>4</v>
-      </c>
-      <c r="BZ118" s="3">
-        <v>9.6853333333333342</v>
-      </c>
-    </row>
-    <row r="119" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
-        <v>30</v>
-      </c>
-      <c r="B119" s="2">
-        <v>1</v>
-      </c>
-      <c r="C119" s="2">
-        <v>6</v>
-      </c>
-      <c r="D119" s="2">
-        <v>0</v>
-      </c>
-      <c r="E119" s="2">
-        <v>1</v>
-      </c>
-      <c r="F119" s="2">
-        <v>1</v>
-      </c>
-      <c r="G119" s="2">
-        <v>1</v>
-      </c>
-      <c r="H119" s="2">
-        <v>1</v>
-      </c>
-      <c r="I119" s="2">
-        <v>1</v>
-      </c>
-      <c r="J119" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="K119" s="2">
-        <v>4</v>
-      </c>
-      <c r="L119" s="2">
-        <v>1</v>
-      </c>
-      <c r="M119" s="2">
-        <v>1</v>
-      </c>
-      <c r="N119" s="2">
-        <v>0</v>
-      </c>
-      <c r="O119" s="2">
-        <v>6</v>
-      </c>
-      <c r="P119" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q119" s="2">
-        <v>4</v>
-      </c>
-      <c r="R119" s="2">
-        <v>3</v>
-      </c>
-      <c r="S119" s="2">
-        <v>4</v>
-      </c>
-      <c r="T119" s="2">
-        <v>3</v>
-      </c>
-      <c r="U119" s="2">
-        <v>3</v>
-      </c>
-      <c r="V119" s="2">
-        <v>2</v>
-      </c>
-      <c r="W119" s="2">
-        <v>6</v>
-      </c>
-      <c r="X119" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y119" s="2">
-        <v>3</v>
-      </c>
-      <c r="Z119" s="2">
-        <v>3</v>
-      </c>
-      <c r="AA119" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB119" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC119" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD119" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE119" s="2">
-        <v>2</v>
-      </c>
-      <c r="AF119" s="2">
-        <v>6</v>
-      </c>
-      <c r="AG119" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH119" s="2">
-        <v>3</v>
-      </c>
-      <c r="AI119" s="2">
-        <v>4</v>
-      </c>
-      <c r="AJ119" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK119" s="2">
-        <v>3</v>
-      </c>
-      <c r="AL119" s="2">
-        <v>4</v>
-      </c>
-      <c r="AM119" s="2">
-        <v>6</v>
-      </c>
-      <c r="AN119" s="2">
-        <v>5</v>
-      </c>
-      <c r="AO119" s="2">
-        <v>6</v>
-      </c>
-      <c r="AP119" s="2">
-        <v>7</v>
-      </c>
-      <c r="AQ119" s="2">
-        <v>6</v>
-      </c>
-      <c r="AR119" s="2">
-        <v>6</v>
-      </c>
-      <c r="AS119" s="2">
-        <v>6</v>
-      </c>
-      <c r="AT119" s="2">
-        <v>4</v>
-      </c>
-      <c r="AU119" s="2">
-        <v>5</v>
-      </c>
-      <c r="AV119" s="2">
-        <v>4</v>
-      </c>
-      <c r="AW119" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX119" s="2">
-        <v>6</v>
-      </c>
-      <c r="AY119" s="2">
-        <v>4</v>
-      </c>
-      <c r="AZ119" s="2">
-        <v>7</v>
-      </c>
-      <c r="BA119" s="2">
-        <v>4</v>
-      </c>
-      <c r="BB119" s="2">
-        <v>7</v>
-      </c>
-      <c r="BC119" s="2">
-        <v>6</v>
-      </c>
-      <c r="BD119" s="2">
-        <v>5</v>
-      </c>
-      <c r="BE119" s="2">
-        <v>3</v>
-      </c>
-      <c r="BF119" s="2">
-        <v>1</v>
-      </c>
-      <c r="BG119" s="2">
-        <v>6</v>
-      </c>
-      <c r="BH119" s="2">
-        <v>5</v>
-      </c>
-      <c r="BI119" s="2">
-        <v>7</v>
-      </c>
-      <c r="BJ119" s="2">
-        <v>3</v>
-      </c>
-      <c r="BK119" s="2">
-        <v>4</v>
-      </c>
-      <c r="BL119" s="2">
-        <v>1</v>
-      </c>
-      <c r="BM119" s="2">
-        <v>5</v>
-      </c>
-      <c r="BN119" s="2">
-        <v>5</v>
-      </c>
-      <c r="BO119" s="2">
-        <v>6</v>
-      </c>
-      <c r="BP119" s="2">
-        <v>6</v>
-      </c>
-      <c r="BQ119" s="2">
-        <v>5</v>
-      </c>
-      <c r="BR119" s="2">
-        <v>7</v>
-      </c>
-      <c r="BS119" s="2">
-        <v>6</v>
-      </c>
-      <c r="BT119" s="2">
-        <v>4</v>
-      </c>
-      <c r="BU119" s="2">
-        <v>3</v>
-      </c>
-      <c r="BV119" s="2">
-        <v>4</v>
-      </c>
-      <c r="BW119" s="2">
-        <v>3</v>
-      </c>
-      <c r="BX119" s="2">
-        <v>4</v>
-      </c>
-      <c r="BY119" s="2">
-        <v>5</v>
-      </c>
-      <c r="BZ119" s="3">
-        <v>15.766500000000001</v>
-      </c>
-    </row>
-    <row r="120" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
-        <v>22</v>
-      </c>
-      <c r="B120" s="2">
-        <v>2</v>
-      </c>
-      <c r="C120" s="2">
-        <v>4</v>
-      </c>
-      <c r="D120" s="2">
-        <v>3</v>
-      </c>
-      <c r="E120" s="2">
-        <v>1</v>
-      </c>
-      <c r="F120" s="2">
-        <v>3</v>
-      </c>
-      <c r="G120" s="2">
-        <v>1</v>
-      </c>
-      <c r="H120" s="2">
-        <v>1</v>
-      </c>
-      <c r="I120" s="2">
-        <v>2</v>
-      </c>
-      <c r="J120" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K120" s="2">
-        <v>7</v>
-      </c>
-      <c r="L120" s="2">
-        <v>0</v>
-      </c>
-      <c r="M120" s="2">
-        <v>0</v>
-      </c>
-      <c r="N120" s="2">
-        <v>1</v>
-      </c>
-      <c r="O120" s="2">
-        <v>6</v>
-      </c>
-      <c r="P120" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q120" s="2">
-        <v>3</v>
-      </c>
-      <c r="R120" s="2">
-        <v>4</v>
-      </c>
-      <c r="S120" s="2">
-        <v>4</v>
-      </c>
-      <c r="T120" s="2">
-        <v>3</v>
-      </c>
-      <c r="U120" s="2">
-        <v>3</v>
-      </c>
-      <c r="V120" s="2">
-        <v>2</v>
-      </c>
-      <c r="W120" s="2">
-        <v>5</v>
-      </c>
-      <c r="X120" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y120" s="2">
-        <v>4</v>
-      </c>
-      <c r="Z120" s="2">
-        <v>4</v>
-      </c>
-      <c r="AA120" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB120" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC120" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD120" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE120" s="2">
-        <v>3</v>
-      </c>
-      <c r="AF120" s="2">
-        <v>5</v>
-      </c>
-      <c r="AG120" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH120" s="2">
-        <v>3</v>
-      </c>
-      <c r="AI120" s="2">
-        <v>4</v>
-      </c>
-      <c r="AJ120" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK120" s="2">
-        <v>6</v>
-      </c>
-      <c r="AL120" s="2">
-        <v>4</v>
-      </c>
-      <c r="AM120" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN120" s="2">
-        <v>7</v>
-      </c>
-      <c r="AO120" s="2">
-        <v>7</v>
-      </c>
-      <c r="AP120" s="2">
-        <v>6</v>
-      </c>
-      <c r="AQ120" s="2">
-        <v>7</v>
-      </c>
-      <c r="AR120" s="2">
-        <v>7</v>
-      </c>
-      <c r="AS120" s="2">
-        <v>7</v>
-      </c>
-      <c r="AT120" s="2">
-        <v>6</v>
-      </c>
-      <c r="AU120" s="2">
-        <v>6</v>
-      </c>
-      <c r="AV120" s="2">
-        <v>6</v>
-      </c>
-      <c r="AW120" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX120" s="2">
-        <v>6</v>
-      </c>
-      <c r="AY120" s="2">
-        <v>6</v>
-      </c>
-      <c r="AZ120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BA120" s="2">
-        <v>6</v>
-      </c>
-      <c r="BB120" s="2">
-        <v>6</v>
-      </c>
-      <c r="BC120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BD120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BE120" s="2">
-        <v>6</v>
-      </c>
-      <c r="BF120" s="2">
-        <v>7</v>
-      </c>
-      <c r="BG120" s="2">
-        <v>3</v>
-      </c>
-      <c r="BH120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BI120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BJ120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BK120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BL120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BM120" s="2">
-        <v>3</v>
-      </c>
-      <c r="BN120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BO120" s="2">
-        <v>5</v>
-      </c>
-      <c r="BP120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BQ120" s="2">
-        <v>6</v>
-      </c>
-      <c r="BR120" s="2">
-        <v>6</v>
-      </c>
-      <c r="BS120" s="2">
-        <v>6</v>
-      </c>
-      <c r="BT120" s="2">
-        <v>3</v>
-      </c>
-      <c r="BU120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BV120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BW120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BX120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BY120" s="2">
-        <v>4</v>
-      </c>
-      <c r="BZ120" s="3">
-        <v>23.423500000000001</v>
-      </c>
-    </row>
-    <row r="121" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
-        <v>39</v>
-      </c>
-      <c r="B121" s="2">
-        <v>2</v>
-      </c>
-      <c r="C121" s="2">
-        <v>6</v>
-      </c>
-      <c r="D121" s="2">
-        <v>24</v>
-      </c>
-      <c r="E121" s="2">
-        <v>1</v>
-      </c>
-      <c r="F121" s="2">
-        <v>3</v>
-      </c>
-      <c r="G121" s="2">
-        <v>1</v>
-      </c>
-      <c r="H121" s="2">
-        <v>1</v>
-      </c>
-      <c r="I121" s="2">
-        <v>1</v>
-      </c>
-      <c r="J121" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K121" s="2">
-        <v>0</v>
-      </c>
-      <c r="L121" s="2">
-        <v>0</v>
-      </c>
-      <c r="M121" s="2">
-        <v>1</v>
-      </c>
-      <c r="N121" s="2">
-        <v>0</v>
-      </c>
-      <c r="O121" s="2">
-        <v>6</v>
-      </c>
-      <c r="P121" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q121" s="2">
-        <v>4</v>
-      </c>
-      <c r="R121" s="2">
-        <v>5</v>
-      </c>
-      <c r="S121" s="2">
-        <v>5</v>
-      </c>
-      <c r="T121" s="2">
-        <v>4</v>
-      </c>
-      <c r="U121" s="2">
-        <v>4</v>
-      </c>
-      <c r="V121" s="2">
-        <v>3</v>
-      </c>
-      <c r="W121" s="2">
-        <v>7</v>
-      </c>
-      <c r="X121" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y121" s="2">
-        <v>3</v>
-      </c>
-      <c r="Z121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AA121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AB121" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC121" s="2">
-        <v>5</v>
-      </c>
-      <c r="AD121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AE121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AF121" s="2">
-        <v>7</v>
-      </c>
-      <c r="AG121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AH121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AI121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AJ121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AL121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AM121" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN121" s="2">
-        <v>7</v>
-      </c>
-      <c r="AO121" s="2">
-        <v>7</v>
-      </c>
-      <c r="AP121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AQ121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AR121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AS121" s="2">
-        <v>7</v>
-      </c>
-      <c r="AT121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AU121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AV121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AW121" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AY121" s="2">
-        <v>6</v>
-      </c>
-      <c r="AZ121" s="2">
-        <v>7</v>
-      </c>
-      <c r="BA121" s="2">
-        <v>7</v>
-      </c>
-      <c r="BB121" s="2">
-        <v>7</v>
-      </c>
-      <c r="BC121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BD121" s="2">
-        <v>7</v>
-      </c>
-      <c r="BE121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BF121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BG121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BH121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BI121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BJ121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BK121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BL121" s="2">
-        <v>3</v>
-      </c>
-      <c r="BM121" s="2">
-        <v>3</v>
-      </c>
-      <c r="BN121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BO121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BP121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BQ121" s="2">
-        <v>7</v>
-      </c>
-      <c r="BR121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BS121" s="2">
-        <v>6</v>
-      </c>
-      <c r="BT121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BU121" s="2">
-        <v>3</v>
-      </c>
-      <c r="BV121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BW121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BX121" s="2">
-        <v>5</v>
-      </c>
-      <c r="BY121" s="2">
-        <v>4</v>
-      </c>
-      <c r="BZ121" s="3">
-        <v>16.439499999999999</v>
-      </c>
-    </row>
-    <row r="122" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
-        <v>27</v>
-      </c>
-      <c r="B122" s="2">
-        <v>2</v>
-      </c>
-      <c r="C122" s="2">
-        <v>6</v>
-      </c>
-      <c r="D122" s="2">
-        <v>9</v>
-      </c>
-      <c r="E122" s="2">
-        <v>1</v>
-      </c>
-      <c r="F122" s="2">
-        <v>3</v>
-      </c>
-      <c r="G122" s="2">
-        <v>4</v>
-      </c>
-      <c r="H122" s="2">
-        <v>1</v>
-      </c>
-      <c r="I122" s="2">
-        <v>1</v>
-      </c>
-      <c r="J122" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K122" s="2">
-        <v>2</v>
-      </c>
-      <c r="L122" s="2">
-        <v>1</v>
-      </c>
-      <c r="M122" s="2">
-        <v>1</v>
-      </c>
-      <c r="N122" s="2">
-        <v>0</v>
-      </c>
-      <c r="O122" s="2">
-        <v>6</v>
-      </c>
-      <c r="P122" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q122" s="2">
-        <v>6</v>
-      </c>
-      <c r="R122" s="2">
-        <v>6</v>
-      </c>
-      <c r="S122" s="2">
-        <v>6</v>
-      </c>
-      <c r="T122" s="2">
-        <v>3</v>
-      </c>
-      <c r="U122" s="2">
-        <v>5</v>
-      </c>
-      <c r="V122" s="2">
-        <v>5</v>
-      </c>
-      <c r="W122" s="2">
-        <v>7</v>
-      </c>
-      <c r="X122" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y122" s="2">
-        <v>4</v>
-      </c>
-      <c r="Z122" s="2">
-        <v>5</v>
-      </c>
-      <c r="AA122" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AC122" s="2">
-        <v>4</v>
-      </c>
-      <c r="AD122" s="2">
-        <v>3</v>
-      </c>
-      <c r="AE122" s="2">
-        <v>4</v>
-      </c>
-      <c r="AF122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AG122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AH122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AI122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AJ122" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AL122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AM122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AO122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AP122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AQ122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AR122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AS122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AT122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AU122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AV122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AW122" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX122" s="2">
-        <v>6</v>
-      </c>
-      <c r="AY122" s="2">
-        <v>7</v>
-      </c>
-      <c r="AZ122" s="2">
-        <v>6</v>
-      </c>
-      <c r="BA122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BB122" s="2">
-        <v>7</v>
-      </c>
-      <c r="BC122" s="2">
-        <v>7</v>
-      </c>
-      <c r="BD122" s="2">
-        <v>7</v>
-      </c>
-      <c r="BE122" s="2">
-        <v>2</v>
-      </c>
-      <c r="BF122" s="2">
-        <v>4</v>
-      </c>
-      <c r="BG122" s="2">
-        <v>3</v>
-      </c>
-      <c r="BH122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BI122" s="2">
-        <v>7</v>
-      </c>
-      <c r="BJ122" s="2">
-        <v>7</v>
-      </c>
-      <c r="BK122" s="2">
-        <v>3</v>
-      </c>
-      <c r="BL122" s="2">
-        <v>1</v>
-      </c>
-      <c r="BM122" s="2">
-        <v>4</v>
-      </c>
-      <c r="BN122" s="2">
-        <v>4</v>
-      </c>
-      <c r="BO122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BP122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BQ122" s="2">
-        <v>7</v>
-      </c>
-      <c r="BR122" s="2">
-        <v>6</v>
-      </c>
-      <c r="BS122" s="2">
-        <v>6</v>
-      </c>
-      <c r="BT122" s="2">
-        <v>3</v>
-      </c>
-      <c r="BU122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BV122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BW122" s="2">
-        <v>4</v>
-      </c>
-      <c r="BX122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BY122" s="2">
-        <v>5</v>
-      </c>
-      <c r="BZ122" s="3">
-        <v>13.94</v>
-      </c>
-    </row>
-    <row r="123" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="2">
-        <v>31</v>
-      </c>
-      <c r="B123" s="2">
-        <v>2</v>
-      </c>
-      <c r="C123" s="2">
-        <v>6</v>
-      </c>
-      <c r="D123" s="2">
-        <v>6</v>
-      </c>
-      <c r="E123" s="2">
-        <v>1</v>
-      </c>
-      <c r="F123" s="2">
-        <v>3</v>
-      </c>
-      <c r="G123" s="2">
-        <v>2</v>
-      </c>
-      <c r="H123" s="2">
-        <v>1</v>
-      </c>
-      <c r="I123" s="2">
-        <v>2</v>
-      </c>
-      <c r="J123" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K123" s="2">
-        <v>6</v>
-      </c>
-      <c r="L123" s="2">
-        <v>1</v>
-      </c>
-      <c r="M123" s="2">
-        <v>1</v>
-      </c>
-      <c r="N123" s="2">
-        <v>0</v>
-      </c>
-      <c r="O123" s="2">
-        <v>6</v>
-      </c>
-      <c r="P123" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q123" s="2">
-        <v>5</v>
-      </c>
-      <c r="R123" s="2">
-        <v>6</v>
-      </c>
-      <c r="S123" s="2">
-        <v>7</v>
-      </c>
-      <c r="T123" s="2">
-        <v>1</v>
-      </c>
-      <c r="U123" s="2">
-        <v>1</v>
-      </c>
-      <c r="V123" s="2">
-        <v>5</v>
-      </c>
-      <c r="W123" s="2">
-        <v>7</v>
-      </c>
-      <c r="X123" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y123" s="2">
-        <v>5</v>
-      </c>
-      <c r="Z123" s="2">
-        <v>3</v>
-      </c>
-      <c r="AA123" s="2">
-        <v>3</v>
-      </c>
-      <c r="AB123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AC123" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD123" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE123" s="2">
-        <v>3</v>
-      </c>
-      <c r="AF123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AG123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AH123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AI123" s="2">
-        <v>3</v>
-      </c>
-      <c r="AJ123" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AL123" s="2">
-        <v>4</v>
-      </c>
-      <c r="AM123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AO123" s="2">
-        <v>4</v>
-      </c>
-      <c r="AP123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AQ123" s="2">
-        <v>1</v>
-      </c>
-      <c r="AR123" s="2">
-        <v>4</v>
-      </c>
-      <c r="AS123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AT123" s="2">
-        <v>6</v>
-      </c>
-      <c r="AU123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AV123" s="2">
-        <v>7</v>
-      </c>
-      <c r="AW123" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX123" s="2">
-        <v>5</v>
-      </c>
-      <c r="AY123" s="2">
-        <v>6</v>
-      </c>
-      <c r="AZ123" s="2">
-        <v>7</v>
-      </c>
-      <c r="BA123" s="2">
-        <v>6</v>
-      </c>
-      <c r="BB123" s="2">
-        <v>7</v>
-      </c>
-      <c r="BC123" s="2">
-        <v>6</v>
-      </c>
-      <c r="BD123" s="2">
-        <v>2</v>
-      </c>
-      <c r="BE123" s="2">
-        <v>4</v>
-      </c>
-      <c r="BF123" s="2">
-        <v>3</v>
-      </c>
-      <c r="BG123" s="2">
-        <v>2</v>
-      </c>
-      <c r="BH123" s="2">
-        <v>6</v>
-      </c>
-      <c r="BI123" s="2">
-        <v>7</v>
-      </c>
-      <c r="BJ123" s="2">
-        <v>4</v>
-      </c>
-      <c r="BK123" s="2">
-        <v>4</v>
-      </c>
-      <c r="BL123" s="2">
-        <v>1</v>
-      </c>
-      <c r="BM123" s="2">
-        <v>2</v>
-      </c>
-      <c r="BN123" s="2">
-        <v>2</v>
-      </c>
-      <c r="BO123" s="2">
-        <v>4</v>
-      </c>
-      <c r="BP123" s="2">
-        <v>1</v>
-      </c>
-      <c r="BQ123" s="2">
-        <v>7</v>
-      </c>
-      <c r="BR123" s="2">
-        <v>6</v>
-      </c>
-      <c r="BS123" s="2">
-        <v>7</v>
-      </c>
-      <c r="BT123" s="2">
-        <v>3</v>
-      </c>
-      <c r="BU123" s="2">
-        <v>3</v>
-      </c>
-      <c r="BV123" s="2">
-        <v>5</v>
-      </c>
-      <c r="BW123" s="2">
-        <v>3</v>
-      </c>
-      <c r="BX123" s="2">
-        <v>5</v>
-      </c>
-      <c r="BY123" s="2">
-        <v>5</v>
-      </c>
-      <c r="BZ123" s="3">
-        <v>26.33966666666667</v>
-      </c>
-    </row>
-    <row r="124" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="2">
-        <v>35</v>
-      </c>
-      <c r="B124" s="2">
-        <v>2</v>
-      </c>
-      <c r="C124" s="2">
-        <v>6</v>
-      </c>
-      <c r="D124" s="2">
-        <v>9</v>
-      </c>
-      <c r="E124" s="2">
-        <v>1</v>
-      </c>
-      <c r="F124" s="2">
-        <v>1</v>
-      </c>
-      <c r="G124" s="2">
-        <v>4</v>
-      </c>
-      <c r="H124" s="2">
-        <v>1</v>
-      </c>
-      <c r="I124" s="2">
-        <v>1</v>
-      </c>
-      <c r="J124" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K124" s="2">
-        <v>9</v>
-      </c>
-      <c r="L124" s="2">
-        <v>1</v>
-      </c>
-      <c r="M124" s="2">
-        <v>0</v>
-      </c>
-      <c r="N124" s="2">
-        <v>1</v>
-      </c>
-      <c r="O124" s="2">
-        <v>6</v>
-      </c>
-      <c r="P124" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q124" s="2">
-        <v>5</v>
-      </c>
-      <c r="R124" s="2">
-        <v>6</v>
-      </c>
-      <c r="S124" s="2">
-        <v>7</v>
-      </c>
-      <c r="T124" s="2">
-        <v>3</v>
-      </c>
-      <c r="U124" s="2">
-        <v>4</v>
-      </c>
-      <c r="V124" s="2">
-        <v>5</v>
-      </c>
-      <c r="W124" s="2">
-        <v>7</v>
-      </c>
-      <c r="X124" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y124" s="2">
-        <v>5</v>
-      </c>
-      <c r="Z124" s="2">
-        <v>5</v>
-      </c>
-      <c r="AA124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AB124" s="2">
-        <v>7</v>
-      </c>
-      <c r="AC124" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD124" s="2">
-        <v>4</v>
-      </c>
-      <c r="AE124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AF124" s="2">
-        <v>7</v>
-      </c>
-      <c r="AG124" s="2">
-        <v>7</v>
-      </c>
-      <c r="AH124" s="2">
-        <v>5</v>
-      </c>
-      <c r="AI124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AJ124" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK124" s="2">
-        <v>5</v>
-      </c>
-      <c r="AL124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AM124" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AO124" s="2">
-        <v>5</v>
-      </c>
-      <c r="AP124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AQ124" s="2">
-        <v>7</v>
-      </c>
-      <c r="AR124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AS124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AT124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AU124" s="2">
-        <v>5</v>
-      </c>
-      <c r="AV124" s="2">
-        <v>7</v>
-      </c>
-      <c r="AW124" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX124" s="2">
-        <v>7</v>
-      </c>
-      <c r="AY124" s="2">
-        <v>6</v>
-      </c>
-      <c r="AZ124" s="2">
-        <v>5</v>
-      </c>
-      <c r="BA124" s="2">
-        <v>7</v>
-      </c>
-      <c r="BB124" s="2">
-        <v>5</v>
-      </c>
-      <c r="BC124" s="2">
-        <v>7</v>
-      </c>
-      <c r="BD124" s="2">
-        <v>6</v>
-      </c>
-      <c r="BE124" s="2">
-        <v>5</v>
-      </c>
-      <c r="BF124" s="2">
-        <v>6</v>
-      </c>
-      <c r="BG124" s="2">
-        <v>2</v>
-      </c>
-      <c r="BH124" s="2">
-        <v>2</v>
-      </c>
-      <c r="BI124" s="2">
-        <v>3</v>
-      </c>
-      <c r="BJ124" s="2">
-        <v>5</v>
-      </c>
-      <c r="BK124" s="2">
-        <v>6</v>
-      </c>
-      <c r="BL124" s="2">
-        <v>6</v>
-      </c>
-      <c r="BM124" s="2">
-        <v>3</v>
-      </c>
-      <c r="BN124" s="2">
-        <v>3</v>
-      </c>
-      <c r="BO124" s="2">
-        <v>5</v>
-      </c>
-      <c r="BP124" s="2">
-        <v>4</v>
-      </c>
-      <c r="BQ124" s="2">
-        <v>7</v>
-      </c>
-      <c r="BR124" s="2">
-        <v>6</v>
-      </c>
-      <c r="BS124" s="2">
-        <v>7</v>
-      </c>
-      <c r="BT124" s="2">
-        <v>5</v>
-      </c>
-      <c r="BU124" s="2">
-        <v>4</v>
-      </c>
-      <c r="BV124" s="2">
-        <v>4</v>
-      </c>
-      <c r="BW124" s="2">
-        <v>4</v>
-      </c>
-      <c r="BX124" s="2">
-        <v>5</v>
-      </c>
-      <c r="BY124" s="2">
-        <v>4</v>
-      </c>
-      <c r="BZ124" s="3">
-        <v>10.832833333333333</v>
-      </c>
-    </row>
-    <row r="125" spans="1:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="2">
-        <v>32</v>
-      </c>
-      <c r="B125" s="2">
-        <v>2</v>
-      </c>
-      <c r="C125" s="2">
-        <v>6</v>
-      </c>
-      <c r="D125" s="2">
-        <v>7</v>
-      </c>
-      <c r="E125" s="2">
-        <v>1</v>
-      </c>
-      <c r="F125" s="2">
-        <v>1</v>
-      </c>
-      <c r="G125" s="2">
-        <v>4</v>
-      </c>
-      <c r="H125" s="2">
-        <v>1</v>
-      </c>
-      <c r="I125" s="2">
-        <v>1</v>
-      </c>
-      <c r="J125" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K125" s="2">
-        <v>12</v>
-      </c>
-      <c r="L125" s="2">
-        <v>1</v>
-      </c>
-      <c r="M125" s="2">
-        <v>1</v>
-      </c>
-      <c r="N125" s="2">
-        <v>1</v>
-      </c>
-      <c r="O125" s="2">
-        <v>6</v>
-      </c>
-      <c r="P125" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q125" s="2">
-        <v>3</v>
-      </c>
-      <c r="R125" s="2">
-        <v>5</v>
-      </c>
-      <c r="S125" s="2">
-        <v>1</v>
-      </c>
-      <c r="T125" s="2">
-        <v>3</v>
-      </c>
-      <c r="U125" s="2">
-        <v>7</v>
-      </c>
-      <c r="V125" s="2">
-        <v>7</v>
-      </c>
-      <c r="W125" s="2">
-        <v>6</v>
-      </c>
-      <c r="X125" s="2">
-        <v>4</v>
-      </c>
-      <c r="Y125" s="2">
-        <v>2</v>
-      </c>
-      <c r="Z125" s="2">
-        <v>6</v>
-      </c>
-      <c r="AA125" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB125" s="2">
-        <v>5</v>
-      </c>
-      <c r="AC125" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD125" s="2">
-        <v>4</v>
-      </c>
-      <c r="AE125" s="2">
-        <v>3</v>
-      </c>
-      <c r="AF125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AG125" s="2">
-        <v>6</v>
-      </c>
-      <c r="AH125" s="2">
-        <v>6</v>
-      </c>
-      <c r="AI125" s="2">
-        <v>3</v>
-      </c>
-      <c r="AJ125" s="2">
-        <v>4</v>
-      </c>
-      <c r="AK125" s="2">
-        <v>2</v>
-      </c>
-      <c r="AL125" s="2">
-        <v>2</v>
-      </c>
-      <c r="AM125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AN125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AO125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AP125" s="2">
-        <v>6</v>
-      </c>
-      <c r="AQ125" s="2">
-        <v>6</v>
-      </c>
-      <c r="AR125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AS125" s="2">
-        <v>5</v>
-      </c>
-      <c r="AT125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AU125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AV125" s="2">
-        <v>7</v>
-      </c>
-      <c r="AW125" s="2">
-        <v>4</v>
-      </c>
-      <c r="AX125" s="2">
-        <v>5</v>
-      </c>
-      <c r="AY125" s="2">
-        <v>6</v>
-      </c>
-      <c r="AZ125" s="2">
-        <v>6</v>
-      </c>
-      <c r="BA125" s="2">
-        <v>6</v>
-      </c>
-      <c r="BB125" s="2">
-        <v>6</v>
-      </c>
-      <c r="BC125" s="2">
-        <v>7</v>
-      </c>
-      <c r="BD125" s="2">
-        <v>6</v>
-      </c>
-      <c r="BE125" s="2">
-        <v>5</v>
-      </c>
-      <c r="BF125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BG125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BH125" s="2">
-        <v>5</v>
-      </c>
-      <c r="BI125" s="2">
-        <v>3</v>
-      </c>
-      <c r="BJ125" s="2">
-        <v>2</v>
-      </c>
-      <c r="BK125" s="2">
-        <v>6</v>
-      </c>
-      <c r="BL125" s="2">
-        <v>2</v>
-      </c>
-      <c r="BM125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BN125" s="2">
-        <v>3</v>
-      </c>
-      <c r="BO125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BP125" s="2">
-        <v>5</v>
-      </c>
-      <c r="BQ125" s="2">
-        <v>7</v>
-      </c>
-      <c r="BR125" s="2">
-        <v>6</v>
-      </c>
-      <c r="BS125" s="2">
-        <v>6</v>
-      </c>
-      <c r="BT125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BU125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BV125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BW125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BX125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BY125" s="2">
-        <v>4</v>
-      </c>
-      <c r="BZ125" s="3">
-        <v>10.610666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>